<commit_message>
incorporated updated coded mex files into the pipeline, pending qa of changes.
</commit_message>
<xml_diff>
--- a/data/coded_segments/zm_3_5.xlsx
+++ b/data/coded_segments/zm_3_5.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Whiting/Repositories/amr-db/data/coded_segments_rename/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D6B4514-8661-204D-9F36-C98A9913893F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3770" uniqueCount="1023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="1028">
   <si>
     <t>Color</t>
   </si>
@@ -3175,19 +3171,34 @@
     <t>6/8/18 13:03:00</t>
   </si>
   <si>
-    <t>23761</t>
-  </si>
-  <si>
-    <t>1: 230|734</t>
-  </si>
-  <si>
-    <t>1: 409|767</t>
+    <t>1: 120</t>
+  </si>
+  <si>
+    <t>1: 139</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Sonia</t>
+  </si>
+  <si>
+    <t>10/29/18 12:12:00</t>
+  </si>
+  <si>
+    <t>1: 2292</t>
+  </si>
+  <si>
+    <t>1: 2301</t>
+  </si>
+  <si>
+    <t>10/30/18 15:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3337,10 +3348,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3363,7 +3377,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3402,52 +3422,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="904875"/>
-          <a:ext cx="1219370" cy="1219370"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>376</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3333750</xdr:colOff>
-      <xdr:row>377</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -3485,7 +3472,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -3497,7 +3484,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -3514,9 +3501,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -3544,14 +3531,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -3579,6 +3583,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3730,8 +3751,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M377"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M378"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3788,7 +3809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="90" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -3911,7 +3932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -3952,7 +3973,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -3993,7 +4014,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -4977,7 +4998,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
@@ -5018,7 +5039,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>13</v>
       </c>
@@ -5098,7 +5119,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>13</v>
       </c>
@@ -7066,7 +7087,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>13</v>
       </c>
@@ -7107,7 +7128,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>13</v>
       </c>
@@ -7230,7 +7251,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="112" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="120" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>13</v>
       </c>
@@ -7271,7 +7292,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>13</v>
       </c>
@@ -7804,7 +7825,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>13</v>
       </c>
@@ -8337,7 +8358,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>13</v>
       </c>
@@ -9649,7 +9670,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>13</v>
       </c>
@@ -9772,7 +9793,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>13</v>
       </c>
@@ -12109,7 +12130,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
         <v>13</v>
       </c>
@@ -12150,7 +12171,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
         <v>13</v>
       </c>
@@ -12191,7 +12212,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="98" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
         <v>13</v>
       </c>
@@ -12232,7 +12253,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
         <v>13</v>
       </c>
@@ -12273,7 +12294,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
         <v>13</v>
       </c>
@@ -12314,7 +12335,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A210" s="6" t="s">
         <v>13</v>
       </c>
@@ -12355,7 +12376,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
         <v>13</v>
       </c>
@@ -12437,7 +12458,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="213" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
         <v>13</v>
       </c>
@@ -12519,7 +12540,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
         <v>13</v>
       </c>
@@ -13216,7 +13237,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
         <v>13</v>
       </c>
@@ -13380,7 +13401,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A236" s="6" t="s">
         <v>13</v>
       </c>
@@ -13462,7 +13483,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="238" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A238" s="6" t="s">
         <v>13</v>
       </c>
@@ -15348,7 +15369,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="284" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A284" s="6" t="s">
         <v>13</v>
       </c>
@@ -15635,7 +15656,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="291" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A291" s="6" t="s">
         <v>13</v>
       </c>
@@ -15676,7 +15697,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="292" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A292" s="6" t="s">
         <v>13</v>
       </c>
@@ -15717,7 +15738,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="293" spans="1:13" ht="98" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A293" s="6" t="s">
         <v>13</v>
       </c>
@@ -15758,7 +15779,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="294" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A294" s="6" t="s">
         <v>13</v>
       </c>
@@ -15799,7 +15820,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="295" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A295" s="6" t="s">
         <v>13</v>
       </c>
@@ -15840,7 +15861,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="296" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A296" s="6" t="s">
         <v>13</v>
       </c>
@@ -16494,7 +16515,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="312" spans="1:13" ht="70" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A312" s="6" t="s">
         <v>13</v>
       </c>
@@ -16535,7 +16556,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="313" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A313" s="6" t="s">
         <v>13</v>
       </c>
@@ -16617,7 +16638,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="315" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A315" s="6" t="s">
         <v>13</v>
       </c>
@@ -16658,7 +16679,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="316" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A316" s="6" t="s">
         <v>13</v>
       </c>
@@ -16699,7 +16720,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="317" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A317" s="6" t="s">
         <v>13</v>
       </c>
@@ -16740,7 +16761,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="318" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A318" s="6" t="s">
         <v>13</v>
       </c>
@@ -16781,7 +16802,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="319" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A319" s="6" t="s">
         <v>13</v>
       </c>
@@ -16822,7 +16843,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="320" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A320" s="6" t="s">
         <v>13</v>
       </c>
@@ -17355,7 +17376,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="333" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A333" s="6" t="s">
         <v>13</v>
       </c>
@@ -17437,7 +17458,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="335" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A335" s="6" t="s">
         <v>13</v>
       </c>
@@ -17806,7 +17827,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="344" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A344" s="6" t="s">
         <v>13</v>
       </c>
@@ -17929,7 +17950,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="347" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A347" s="6" t="s">
         <v>13</v>
       </c>
@@ -18093,7 +18114,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="351" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A351" s="6" t="s">
         <v>13</v>
       </c>
@@ -18626,7 +18647,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="364" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A364" s="6" t="s">
         <v>13</v>
       </c>
@@ -18749,7 +18770,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="367" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A367" s="6" t="s">
         <v>13</v>
       </c>
@@ -18995,7 +19016,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="373" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A373" s="6" t="s">
         <v>13</v>
       </c>
@@ -19036,7 +19057,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="374" spans="1:13" ht="42" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A374" s="6" t="s">
         <v>13</v>
       </c>
@@ -19077,7 +19098,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="375" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A375" s="6" t="s">
         <v>13</v>
       </c>
@@ -19118,7 +19139,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="376" spans="1:13" ht="56" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A376" s="6" t="s">
         <v>13</v>
       </c>
@@ -19159,7 +19180,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="377" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A377" s="6" t="s">
         <v>13</v>
       </c>
@@ -19170,32 +19191,75 @@
         <v>15</v>
       </c>
       <c r="D377" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E377" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F377" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="E377" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F377" s="1" t="s">
+      <c r="G377" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="G377" s="1" t="s">
+      <c r="H377" s="3">
+        <v>0</v>
+      </c>
+      <c r="I377" s="2" t="s">
         <v>1022</v>
       </c>
-      <c r="H377" s="3">
-        <v>0</v>
-      </c>
-      <c r="I377" s="1"/>
       <c r="J377" s="3">
-        <v>13974</v>
+        <v>20</v>
       </c>
       <c r="K377" s="4">
-        <v>0.41362900000000002</v>
+        <v>6.1873999999999998E-2</v>
       </c>
       <c r="L377" s="1" t="s">
-        <v>576</v>
+        <v>1023</v>
       </c>
       <c r="M377" s="1" t="s">
-        <v>1019</v>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="378" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A378" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E378" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H378" s="3">
+        <v>0</v>
+      </c>
+      <c r="I378" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J378" s="3">
+        <v>10</v>
+      </c>
+      <c r="K378" s="4">
+        <v>3.0936999999999999E-2</v>
+      </c>
+      <c r="L378" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="M378" s="1" t="s">
+        <v>1027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>